<commit_message>
Remove one not needed view
</commit_message>
<xml_diff>
--- a/Diagrams.xlsx
+++ b/Diagrams.xlsx
@@ -5,27 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawo\Desktop\Projects\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dawo\Desktop\Projects\thesis-appendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5258A4-0A9D-4525-8142-4B41B29DD6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F453E6-D132-41D0-A889-8ED46675F024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" activeTab="6" xr2:uid="{31CBB3C6-F395-4396-B14E-C2F50551C2F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="1000" xr2:uid="{31CBB3C6-F395-4396-B14E-C2F50551C2F9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Stage-Role" sheetId="1" r:id="rId1"/>
-    <sheet name="Stage-Experience" sheetId="9" r:id="rId2"/>
-    <sheet name="Stage-TeamSize" sheetId="10" r:id="rId3"/>
-    <sheet name="Stage-CommitImportance" sheetId="11" r:id="rId4"/>
-    <sheet name="Stage-Improvement" sheetId="14" r:id="rId5"/>
-    <sheet name="Stage-UIGrade&lt;C&gt;" sheetId="12" r:id="rId6"/>
-    <sheet name="Stage-Beneficial&lt;C&gt;" sheetId="13" r:id="rId7"/>
-    <sheet name="OneTimer-UIGrade" sheetId="3" r:id="rId8"/>
-    <sheet name="OneTimer-Beneficial" sheetId="4" r:id="rId9"/>
-    <sheet name="OneTimer-Experience" sheetId="5" r:id="rId10"/>
-    <sheet name="OneTimer-TeamSize" sheetId="6" r:id="rId11"/>
-    <sheet name="OneTimer-AverageCommits" sheetId="7" r:id="rId12"/>
-    <sheet name="OneTimer-AverageFile" sheetId="8" r:id="rId13"/>
+    <sheet name="Stage-Experience" sheetId="9" r:id="rId1"/>
+    <sheet name="Stage-TeamSize" sheetId="10" r:id="rId2"/>
+    <sheet name="Stage-CommitImportance" sheetId="11" r:id="rId3"/>
+    <sheet name="Stage-Improvement" sheetId="14" r:id="rId4"/>
+    <sheet name="Stage-UIGrade&lt;C&gt;" sheetId="12" r:id="rId5"/>
+    <sheet name="Stage-Beneficial&lt;C&gt;" sheetId="13" r:id="rId6"/>
+    <sheet name="OneTimer-UIGrade" sheetId="3" r:id="rId7"/>
+    <sheet name="OneTimer-Beneficial" sheetId="4" r:id="rId8"/>
+    <sheet name="OneTimer-Experience" sheetId="5" r:id="rId9"/>
+    <sheet name="OneTimer-TeamSize" sheetId="6" r:id="rId10"/>
+    <sheet name="OneTimer-AverageCommits" sheetId="7" r:id="rId11"/>
+    <sheet name="OneTimer-AverageFile" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,19 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="38">
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Number of testers</t>
-  </si>
-  <si>
-    <t>Software engineer</t>
-  </si>
-  <si>
-    <t>Product Manager</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="34">
   <si>
     <t>Grade</t>
   </si>
@@ -250,43 +237,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t>Role</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t> of</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t> multi-stage</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t> testers</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -320,7 +270,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -328,11 +278,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Stage-Role'!$B$1</c:f>
+              <c:f>'Stage-Experience'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Number of testers</c:v>
+                  <c:v>Years of experience</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -349,36 +299,78 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'Stage-Role'!$A$2:$A$3</c:f>
+              <c:f>'Stage-Experience'!$A$2:$A$10</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>Software engineer</c:v>
+                  <c:v>P1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Product Manager</c:v>
+                  <c:v>P2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>P6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>P7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>P8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>P9</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Stage-Role'!$B$2:$B$3</c:f>
+              <c:f>'Stage-Experience'!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E2B2-4377-A93F-A14ACA234DC7}"/>
+              <c16:uniqueId val="{00000000-F0BE-45DB-9245-B77381377D34}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -390,17 +382,18 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="1371134175"/>
-        <c:axId val="1371104895"/>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1144499455"/>
+        <c:axId val="1144498015"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1371134175"/>
+        <c:axId val="1144499455"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -438,7 +431,7 @@
             <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371104895"/>
+        <c:crossAx val="1144498015"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -446,12 +439,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1371104895"/>
+        <c:axId val="1144498015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -497,7 +490,7 @@
             <a:endParaRPr lang="en-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1371134175"/>
+        <c:crossAx val="1144499455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -547,347 +540,6 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'OneTimer-Experience'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Years of experience</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'OneTimer-Experience'!$A$2:$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>P10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>P11</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>P12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>P13</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>P14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>P15</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>P16</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>P17</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>P18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>P19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>P20</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>P21</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>P22</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'OneTimer-Experience'!$B$2:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0" formatCode="0.0">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="0.0">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="0.0">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A0C3-4384-B830-21F87EF035A0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1483439471"/>
-        <c:axId val="1483438991"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1483439471"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1483438991"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1483438991"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1483439471"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1243,323 +895,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Stage-Experience'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Years of experience</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Stage-Experience'!$A$2:$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>P1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>P2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>P3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>P4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>P5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>P6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>P7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>P8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>P9</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Stage-Experience'!$B$2:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F0BE-45DB-9245-B77381377D34}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1144499455"/>
-        <c:axId val="1144498015"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1144499455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1144498015"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1144498015"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1144499455"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1891,7 +1226,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2238,7 +1573,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2586,7 +1921,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3066,7 +2401,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3555,7 +2890,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3894,7 +3229,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4283,6 +3618,347 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'OneTimer-Experience'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Years of experience</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'OneTimer-Experience'!$A$2:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>P10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>P11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>P12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>P13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>P14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>P15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>P16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>P17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>P18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>P19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>P20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>P21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>P22</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'OneTimer-Experience'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A0C3-4384-B830-21F87EF035A0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1483439471"/>
+        <c:axId val="1483438991"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1483439471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483438991"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1483438991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1483439471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4324,46 +4000,6 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4724,7 +4360,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4928,23 +4564,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -5049,8 +4684,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5182,20 +4817,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -5731,7 +5365,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6234,7 +5868,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6737,7 +6371,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7240,7 +6874,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7743,7 +7377,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8246,7 +7880,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8749,7 +8383,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9252,7 +8886,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9755,530 +9389,27 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0EB73F-320A-BC88-383D-21956A127DE2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E50EA1A-148A-73CF-067B-4B5F1A34A1AD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10300,47 +9431,6 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>119061</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0501490-2418-40BD-5231-C1830E38A79A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10385,47 +9475,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E50EA1A-148A-73CF-067B-4B5F1A34A1AD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>9</xdr:row>
@@ -10463,7 +9512,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10504,7 +9553,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10545,7 +9594,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10586,7 +9635,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10627,7 +9676,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10668,7 +9717,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10689,6 +9738,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA62786-2A18-D038-FC9B-4802A44009C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>119061</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0501490-2418-40BD-5231-C1830E38A79A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -11005,211 +10095,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8A30FA-01EC-40D5-AAC7-6EFDF2847127}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA81794-B8BE-4BA4-9F23-8677A31916B3}">
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8662939A-71B3-45D1-9EB6-8D198806734C}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
-    <sortCondition ref="A2:A14"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88197181-AA05-4A0F-A090-0B0F84B737F2}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -11224,15 +10210,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -11240,7 +10226,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -11248,7 +10234,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="3">
         <v>8</v>
@@ -11256,7 +10242,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>9</v>
@@ -11264,7 +10250,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -11272,7 +10258,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>80</v>
@@ -11280,7 +10266,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -11288,7 +10274,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>6</v>
@@ -11296,15 +10282,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -11312,7 +10298,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>8</v>
@@ -11320,7 +10306,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>24</v>
@@ -11328,7 +10314,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>30</v>
@@ -11343,7 +10329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E7EDFC-1967-40E0-A2A6-7E74C4039781}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -11359,39 +10345,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1095</v>
@@ -11399,7 +10385,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>1825</v>
@@ -11407,23 +10393,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>11315</v>
@@ -11431,23 +10417,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>21900</v>
@@ -11455,15 +10441,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>36500</v>
@@ -11477,7 +10463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC37BB7C-6C77-400A-8D7C-DA1FB8A52B11}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -11492,15 +10478,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3">
         <v>50</v>
@@ -11508,7 +10494,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>10000</v>
@@ -11516,15 +10502,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1000</v>
@@ -11532,7 +10518,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -11540,23 +10526,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
         <v>30</v>
@@ -11564,7 +10550,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>60000</v>
@@ -11572,7 +10558,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>71</v>
@@ -11580,7 +10566,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>800</v>
@@ -11588,18 +10574,18 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -11611,107 +10597,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA81794-B8BE-4BA4-9F23-8677A31916B3}">
-  <dimension ref="A1:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0743CBE-B9FF-40C0-9571-B99F7B0C5442}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -11726,15 +10611,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -11742,7 +10627,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -11750,7 +10635,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -11758,7 +10643,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -11766,7 +10651,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -11774,7 +10659,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -11782,7 +10667,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -11790,7 +10675,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -11798,7 +10683,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -11810,7 +10695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF5B1C5-5E3B-4518-A588-131DC3A16B87}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -11825,15 +10710,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -11841,7 +10726,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>9</v>
@@ -11849,7 +10734,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -11857,7 +10742,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -11865,7 +10750,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -11873,7 +10758,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -11881,7 +10766,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -11889,7 +10774,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>9</v>
@@ -11897,7 +10782,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -11909,7 +10794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F951F6C-DDAF-4FB0-89F3-3DBFD3E7FEA4}">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -11924,15 +10809,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -11940,7 +10825,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -11948,7 +10833,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -11956,7 +10841,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -11964,7 +10849,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -11972,7 +10857,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -11980,7 +10865,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -11988,7 +10873,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -11996,7 +10881,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>7</v>
@@ -12008,7 +10893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7284BA0-9A26-416F-8C11-7FF437056FEB}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -12027,18 +10912,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -12049,7 +10934,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -12060,7 +10945,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="2">
         <v>6.5</v>
@@ -12071,7 +10956,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -12082,7 +10967,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>8</v>
@@ -12093,7 +10978,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -12104,7 +10989,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -12115,7 +11000,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -12126,7 +11011,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -12141,14 +11026,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47C49150-CC8C-46F9-B255-1A74E59B570E}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -12160,18 +11045,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -12182,7 +11067,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -12193,7 +11078,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>6.5</v>
@@ -12204,7 +11089,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -12215,7 +11100,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -12226,7 +11111,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -12237,7 +11122,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -12248,7 +11133,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -12259,13 +11144,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -12274,7 +11159,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDF9D11-0732-477A-95CB-F408D6B8B982}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -12290,10 +11175,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -12340,7 +11225,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -12352,19 +11237,19 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
         <v>17</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -12376,13 +11261,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -12394,16 +11279,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -12419,7 +11304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60B4B936-9758-43A3-B1C1-0764304E9131}">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -12434,10 +11319,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -12466,7 +11351,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -12478,7 +11363,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -12490,19 +11375,19 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -12514,7 +11399,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -12526,10 +11411,10 @@
         <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -12541,7 +11426,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -12553,7 +11438,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -12565,11 +11450,145 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8662939A-71B3-45D1-9EB6-8D198806734C}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+    <sortCondition ref="A2:A14"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>